<commit_message>
Fitting to particular dyads
</commit_message>
<xml_diff>
--- a/Python codes/Dyads/Dyads_parameter_estimations.xlsx
+++ b/Python codes/Dyads/Dyads_parameter_estimations.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Edgar/Documents/DCL-DataAnalysis/Python codes/Dyads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar.andrade\Documents\DCL-DataAnalysis\Python codes\Dyads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DBBB9D-3FB3-0145-8B16-FE57F5BABAF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{05B446A7-314B-5044-B41E-9189BC9A9BEF}"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="25440" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Dyad</t>
   </si>
@@ -54,26 +53,53 @@
     <t>-2 log L</t>
   </si>
   <si>
-    <t>142-263</t>
-  </si>
-  <si>
-    <t>151-962</t>
-  </si>
-  <si>
-    <t>152-727</t>
-  </si>
-  <si>
-    <t>216-713</t>
+    <t>435-261</t>
+  </si>
+  <si>
+    <t>379-897</t>
+  </si>
+  <si>
+    <t>Inside-Outside</t>
+  </si>
+  <si>
+    <t>Left-Right</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>356-137</t>
+  </si>
+  <si>
+    <t>All-Nothing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,17 +122,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,148 +455,211 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39C6DF1-676F-124D-95D2-7EF9B6F3B040}">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>0.72119599999999995</v>
-      </c>
-      <c r="C3">
+      <c r="C3" s="4">
+        <v>0.72116460000000004</v>
+      </c>
+      <c r="D3" s="4">
+        <v>199.9995366</v>
+      </c>
+      <c r="E3" s="4">
+        <v>156.0393</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.11463139999999999</v>
+      </c>
+      <c r="G3" s="4">
+        <v>199.99745179999999</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5.8707985999999996</v>
+      </c>
+      <c r="I3" s="4">
+        <v>10</v>
+      </c>
+      <c r="J3" s="5">
+        <v>54.523600000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.38595819999999997</v>
+      </c>
+      <c r="D4" s="4">
+        <v>199.9999862</v>
+      </c>
+      <c r="E4" s="4">
+        <v>16.039470000000001</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.23991899999999999</v>
+      </c>
+      <c r="G4" s="4">
         <v>200</v>
       </c>
-      <c r="D3">
-        <v>312.07859999999999</v>
-      </c>
-      <c r="E3">
-        <v>0.11463139999999999</v>
-      </c>
-      <c r="F3">
-        <v>199.99745179999999</v>
-      </c>
-      <c r="G3">
-        <v>5.8707985999999996</v>
-      </c>
-      <c r="H3">
+      <c r="H4" s="4">
+        <v>15</v>
+      </c>
+      <c r="I4" s="4">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="J4" s="5">
+        <v>15.717370000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="I3">
-        <v>54.523600000000002</v>
+      <c r="C5" s="4">
+        <v>0.10786270000000001</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.96827419999999997</v>
+      </c>
+      <c r="E5" s="4">
+        <v>25.921489999999999</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.75444319999999998</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.97648069999999998</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="J5" s="4">
+        <v>20.438859999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2.047939E-2</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.88395170000000001</v>
+      </c>
+      <c r="D6" s="4">
+        <v>7.7024844000000003</v>
+      </c>
+      <c r="E6" s="4">
+        <v>63.405709999999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.66561530000000002</v>
+      </c>
+      <c r="G6" s="4">
+        <v>3.8144170000000002E-4</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="I6" s="4">
+        <v>7.1300720000000002</v>
+      </c>
+      <c r="J6" s="4">
+        <v>45.506970000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1.599952E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>0.43276900000000001</v>
-      </c>
-      <c r="C6">
-        <v>1.8267530000000001</v>
-      </c>
-      <c r="D6">
-        <v>192.88149999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>1.2615000000000001</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>356.47919999999999</v>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <f>SUM(E3:E6)</f>
+        <v>261.40597000000002</v>
+      </c>
+      <c r="J8" s="3">
+        <f>SUM(J3:J6)</f>
+        <v>136.18680000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>